<commit_message>
fileReader fix, aktuelle Import Dateien
</commit_message>
<xml_diff>
--- a/ressources/export/EXPORT BOT6 Laufzettel Beispiel vier Schüler.xlsx
+++ b/ressources/export/EXPORT BOT6 Laufzettel Beispiel vier Schüler.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\+++Schule\AE_LF12\Projekt Berufsorientierungstag\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Documents\java_workspace\Eventplanner\ressources\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5703D9F1-668B-49AF-BC46-C602F6C93131}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F43101E-EB2F-48E6-AE06-D41BC4998238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Beispiel 1 DIN A4 Seite" sheetId="3" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="40">
   <si>
     <t>ASS221</t>
   </si>
@@ -1017,8 +1018,8 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1558,7 +1559,596 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA0067F3-8F64-4F5C-9C3C-AC4414CBC990}">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8">
+        <v>103</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8">
+        <v>103</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8">
+        <v>102</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8">
+        <v>102</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="8">
+        <v>107</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="8">
+        <v>106</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="8">
+        <v>112</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="8">
+        <v>113</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="8">
+        <v>103</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="8">
+        <v>103</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="8">
+        <v>102</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="8">
+        <v>102</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="8">
+        <v>107</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="8">
+        <v>106</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="7"/>
+      <c r="F32" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="8">
+        <v>112</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="8">
+        <v>113</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="8">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="dc877d39-ac67-4e82-9042-477ace6c308a">
@@ -1584,15 +2174,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1827,6 +2408,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C40D6BC9-2BFD-4AFA-926B-D88919A76B52}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC737808-C46C-4161-A1F3-7C462EDEDEB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1839,14 +2428,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C40D6BC9-2BFD-4AFA-926B-D88919A76B52}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>